<commit_message>
ajuste notebooks, dependencias y readme
</commit_message>
<xml_diff>
--- a/models/results/DNN_baseline_model_results.xlsx
+++ b/models/results/DNN_baseline_model_results.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -476,31 +476,31 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>MAE</t>
+          <t>MAE [$COP/kWh]</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>MSE</t>
+          <t>MSE [$COP/kWh]</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>RMSE</t>
+          <t>RMSE [$COP/kWh]</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>MAPE</t>
+          <t>MAPE [%]</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -508,7 +508,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E2" t="n">
         <v>60</v>
@@ -518,26 +518,26 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>&lt;keras.src.optimizers.legacy.adam.Adam object at 0x7e1279ce8be0&gt;</t>
+          <t>&lt;keras.src.optimizers.adam.Adam object at 0x0000012D02197B50&gt;</t>
         </is>
       </c>
       <c r="H2" t="n">
         <v>100</v>
       </c>
       <c r="I2" t="n">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="J2" t="n">
-        <v>79.70302451142334</v>
+        <v>69.65316057194121</v>
       </c>
       <c r="K2" t="n">
-        <v>9003.426052322262</v>
+        <v>5636.96271815866</v>
       </c>
       <c r="L2" t="n">
-        <v>94.88638496814104</v>
+        <v>75.07970909745629</v>
       </c>
       <c r="M2" t="n">
-        <v>24.28301385758986</v>
+        <v>42.16618722728619</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajuste final en notebooks y readme
</commit_message>
<xml_diff>
--- a/models/results/DNN_baseline_model_results.xlsx
+++ b/models/results/DNN_baseline_model_results.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -514,30 +514,30 @@
         <v>60</v>
       </c>
       <c r="F2" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>&lt;keras.src.optimizers.adam.Adam object at 0x0000012D02197B50&gt;</t>
+          <t>adam</t>
         </is>
       </c>
       <c r="H2" t="n">
         <v>100</v>
       </c>
       <c r="I2" t="n">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="J2" t="n">
-        <v>69.65316057194121</v>
+        <v>30.4076393629437</v>
       </c>
       <c r="K2" t="n">
-        <v>5636.96271815866</v>
+        <v>1335.891102037011</v>
       </c>
       <c r="L2" t="n">
-        <v>75.07970909745629</v>
+        <v>36.54984407678111</v>
       </c>
       <c r="M2" t="n">
-        <v>42.16618722728619</v>
+        <v>0.1930345932205534</v>
       </c>
     </row>
   </sheetData>

</xml_diff>